<commit_message>
Oprydning og samle i "Spil hele lortet"
</commit_message>
<xml_diff>
--- a/nash-ligevægt_output.xlsx
+++ b/nash-ligevægt_output.xlsx
@@ -483,10 +483,10 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
       <c r="F2">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -503,10 +503,10 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
       <c r="F3">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -523,10 +523,10 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
       <c r="F4">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -543,10 +543,10 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>2.538199269064105</v>
+        <v>22.44744497537364</v>
       </c>
       <c r="F5">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -563,10 +563,10 @@
         <v>47.45339580596996</v>
       </c>
       <c r="E6">
-        <v>29.79474759636823</v>
+        <v>38.08572304239735</v>
       </c>
       <c r="F6">
-        <v>26.41371823387504</v>
+        <v>19.84106529753635</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -583,10 +583,10 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>6.353738935601011</v>
+        <v>1.596407552675339</v>
       </c>
       <c r="F7">
-        <v>4.820376410139755</v>
+        <v>1.596407552675339</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -603,10 +603,10 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
       <c r="F8">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -623,10 +623,10 @@
         <v>11.30771751512249</v>
       </c>
       <c r="E9">
-        <v>12.77191182559202</v>
+        <v>1.596407552675339</v>
       </c>
       <c r="F9">
-        <v>19.91006223634859</v>
+        <v>30.2665840088855</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -643,10 +643,10 @@
         <v>16.16691479588853</v>
       </c>
       <c r="E10">
-        <v>6.383051980952698</v>
+        <v>12.32790358674824</v>
       </c>
       <c r="F10">
-        <v>4.12169762902428</v>
+        <v>1.596407552675339</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -663,10 +663,10 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
       <c r="F11">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -683,10 +683,10 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
       <c r="F12">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -703,10 +703,10 @@
         <v>11.05370299238914</v>
       </c>
       <c r="E13">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
       <c r="F13">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -723,10 +723,10 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
       <c r="F14">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -743,10 +743,10 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
       <c r="F15">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -763,10 +763,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
       <c r="F16">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -783,10 +783,10 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
       <c r="F17">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -803,10 +803,10 @@
         <v>3.714002408323057</v>
       </c>
       <c r="E18">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
       <c r="F18">
-        <v>3.458589291319623</v>
+        <v>1.596407552675339</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -823,10 +823,10 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
       <c r="F19">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -843,10 +843,10 @@
         <v>2.960812269131685</v>
       </c>
       <c r="E20">
-        <v>2.538199269064105</v>
+        <v>1.596407552675339</v>
       </c>
       <c r="F20">
-        <v>4.820376410139755</v>
+        <v>1.596407552675339</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -863,10 +863,10 @@
         <v>7.343454213175142</v>
       </c>
       <c r="E21">
-        <v>6.623560625524499</v>
+        <v>1.596407552675339</v>
       </c>
       <c r="F21">
-        <v>3.458589291319623</v>
+        <v>22.75342229809739</v>
       </c>
     </row>
   </sheetData>

</xml_diff>